<commit_message>
Timesheet - Wednesday match edit
</commit_message>
<xml_diff>
--- a/N17/man/timesheets/OverallTimesheet.xlsx
+++ b/N17/man/timesheets/OverallTimesheet.xlsx
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,14 +628,14 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="O5">
         <v>4</v>
       </c>
       <c r="P5">
         <f>SUM(C5:O5)</f>
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>